<commit_message>
Added new class diagrams
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicolae.andries\IdeaProjects\VVSS\Docs\Lab01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrei 0920\OneDrive\Desktop\VVSS\Proiect\VVSS\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{91CC4B76-21DF-4096-804D-50A5EF88D50E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6935316E-CDF7-444C-A4CD-5A3C5C6FFDC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="5640" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="Tool-basedCodeAnalysis" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1825,8 +1824,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="74">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1836,13 +1835,13 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1861,71 +1860,67 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="8" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="8" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="9" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3200,11 +3195,11 @@
     </row>
     <row r="3" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8"/>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
       <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3376,467 +3371,467 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="12.36328125" style="19" customWidth="1"/>
-    <col min="3" max="3" width="16.36328125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="28" style="19" customWidth="1"/>
-    <col min="5" max="5" width="41.453125" style="19" customWidth="1"/>
-    <col min="6" max="8" width="8.81640625" style="19" customWidth="1"/>
-    <col min="9" max="9" width="21" style="19" customWidth="1"/>
-    <col min="10" max="10" width="14.453125" style="19" customWidth="1"/>
-    <col min="11" max="11" width="8.81640625" style="19" customWidth="1"/>
-    <col min="12" max="16384" width="8.81640625" style="19"/>
+    <col min="1" max="1" width="8.81640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="12.36328125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="16.36328125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="28" style="4" customWidth="1"/>
+    <col min="5" max="5" width="41.453125" style="4" customWidth="1"/>
+    <col min="6" max="8" width="8.81640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="21" style="4" customWidth="1"/>
+    <col min="10" max="10" width="14.453125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="8.81640625" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="8.81640625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20"/>
-      <c r="B1" s="21" t="s">
+      <c r="A1" s="19"/>
+      <c r="B1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="58" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
     </row>
     <row r="2" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="22"/>
-      <c r="B2" s="60" t="s">
+      <c r="A2" s="21"/>
+      <c r="B2" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="25" t="s">
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="J2" s="24" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="25" t="s">
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="25" t="s">
+      <c r="I3" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="25" t="s">
+      <c r="J3" s="24" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="22"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="27" t="s">
+      <c r="A4" s="21"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="62" t="s">
+      <c r="D4" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="63"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="25" t="s">
+      <c r="E4" s="59"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="22"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="27" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="64" t="s">
+      <c r="D5" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="65"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="25" t="s">
+      <c r="E5" s="61"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="25" t="s">
+      <c r="I5" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="25" t="s">
+      <c r="J5" s="24" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="22"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="30" t="s">
+      <c r="A6" s="21"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
     </row>
     <row r="7" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="22"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="30" t="s">
+      <c r="A7" s="21"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
     </row>
     <row r="8" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="22"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
     </row>
     <row r="9" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="23"/>
-      <c r="B9" s="33" t="s">
+      <c r="A9" s="22"/>
+      <c r="B9" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="34" t="s">
+      <c r="E9" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
     </row>
     <row r="10" spans="1:10" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="23"/>
-      <c r="B10" s="35">
+      <c r="A10" s="22"/>
+      <c r="B10" s="34">
         <v>1</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="37" t="s">
+      <c r="E10" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
     </row>
     <row r="11" spans="1:10" ht="58" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="23"/>
-      <c r="B11" s="35">
+      <c r="A11" s="22"/>
+      <c r="B11" s="34">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="37" t="s">
+      <c r="E11" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="28"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
     </row>
     <row r="12" spans="1:10" ht="50.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="23"/>
-      <c r="B12" s="35">
+      <c r="A12" s="22"/>
+      <c r="B12" s="34">
         <v>3</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="36" t="s">
+      <c r="D12" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="37" t="s">
+      <c r="E12" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="28"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
     </row>
     <row r="13" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="23"/>
-      <c r="B13" s="35">
+      <c r="A13" s="22"/>
+      <c r="B13" s="34">
         <f t="shared" ref="B13:B25" si="0">B12+1</f>
         <v>4</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="36" t="s">
+      <c r="D13" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="37" t="s">
+      <c r="E13" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
     </row>
     <row r="14" spans="1:10" ht="46.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="23"/>
-      <c r="B14" s="35">
+      <c r="A14" s="22"/>
+      <c r="B14" s="34">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="36" t="s">
+      <c r="D14" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="37" t="s">
+      <c r="E14" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="28"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
     </row>
     <row r="15" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="23"/>
-      <c r="B15" s="35">
+      <c r="A15" s="22"/>
+      <c r="B15" s="34">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="38"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
     </row>
     <row r="16" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="23"/>
-      <c r="B16" s="35">
+      <c r="A16" s="22"/>
+      <c r="B16" s="34">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
     </row>
     <row r="17" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="23"/>
-      <c r="B17" s="35">
+      <c r="A17" s="22"/>
+      <c r="B17" s="34">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
     </row>
     <row r="18" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="23"/>
-      <c r="B18" s="35">
+      <c r="A18" s="22"/>
+      <c r="B18" s="34">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
     </row>
     <row r="19" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="23"/>
-      <c r="B19" s="35">
+      <c r="A19" s="22"/>
+      <c r="B19" s="34">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
     </row>
     <row r="20" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="23"/>
-      <c r="B20" s="35">
+      <c r="A20" s="22"/>
+      <c r="B20" s="34">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
     </row>
     <row r="21" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="23"/>
-      <c r="B21" s="35">
+      <c r="A21" s="22"/>
+      <c r="B21" s="34">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
     </row>
     <row r="22" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="23"/>
-      <c r="B22" s="35">
+      <c r="A22" s="22"/>
+      <c r="B22" s="34">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
     </row>
     <row r="23" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="23"/>
-      <c r="B23" s="35">
+      <c r="A23" s="22"/>
+      <c r="B23" s="34">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
     </row>
     <row r="24" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="23"/>
-      <c r="B24" s="35">
+      <c r="A24" s="22"/>
+      <c r="B24" s="34">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
     </row>
     <row r="25" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="23"/>
-      <c r="B25" s="35">
+      <c r="A25" s="22"/>
+      <c r="B25" s="34">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
     </row>
     <row r="26" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="22"/>
-      <c r="B26" s="31"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
+      <c r="A26" s="21"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
     </row>
     <row r="27" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="22"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="44" t="s">
+      <c r="A27" s="21"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="D27" s="45"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -3860,484 +3855,486 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="46" customWidth="1"/>
-    <col min="2" max="2" width="12.36328125" style="46" customWidth="1"/>
-    <col min="3" max="3" width="16.36328125" style="46" customWidth="1"/>
-    <col min="4" max="4" width="46.453125" style="46" customWidth="1"/>
-    <col min="5" max="5" width="56" style="46" customWidth="1"/>
-    <col min="6" max="8" width="8.81640625" style="46" customWidth="1"/>
-    <col min="9" max="9" width="22.1796875" style="46" customWidth="1"/>
-    <col min="10" max="11" width="8.81640625" style="46" customWidth="1"/>
-    <col min="12" max="16384" width="8.81640625" style="46"/>
+    <col min="1" max="1" width="8.81640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="12.36328125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="16.36328125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="46.453125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="56" style="4" customWidth="1"/>
+    <col min="6" max="8" width="8.81640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="22.1796875" style="4" customWidth="1"/>
+    <col min="10" max="11" width="8.81640625" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="8.81640625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20"/>
-      <c r="B1" s="21" t="s">
+      <c r="A1" s="19"/>
+      <c r="B1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="58" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
     </row>
     <row r="2" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="22"/>
-      <c r="B2" s="60" t="s">
+      <c r="A2" s="21"/>
+      <c r="B2" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="25" t="s">
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="J2" s="24" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="25" t="s">
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="25" t="s">
+      <c r="I3" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="25" t="s">
+      <c r="J3" s="24" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="22"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="47" t="s">
+      <c r="A4" s="21"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="66" t="s">
+      <c r="D4" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="67"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="25" t="s">
+      <c r="E4" s="63"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="22"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="47" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="70" t="s">
+      <c r="D5" s="66" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="71"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="25" t="s">
+      <c r="E5" s="67"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="25" t="s">
+      <c r="I5" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="25" t="s">
+      <c r="J5" s="24" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="22"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="30" t="s">
+      <c r="A6" s="21"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="68" t="s">
+      <c r="D6" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="57"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
     </row>
     <row r="7" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="22"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="30" t="s">
+      <c r="A7" s="21"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="69">
+      <c r="D7" s="65">
         <v>44991</v>
       </c>
-      <c r="E7" s="57"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
     </row>
     <row r="8" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="22"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
     </row>
     <row r="9" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="23"/>
-      <c r="B9" s="33" t="s">
+      <c r="A9" s="22"/>
+      <c r="B9" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-    </row>
-    <row r="10" spans="1:10" ht="86.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="23"/>
-      <c r="B10" s="35">
+      <c r="F9" s="27"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+    </row>
+    <row r="10" spans="1:10" ht="108" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="22"/>
+      <c r="B10" s="34">
         <v>1</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="49" t="s">
+      <c r="D10" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="49" t="s">
+      <c r="E10" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
     </row>
     <row r="11" spans="1:10" ht="55.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="23"/>
-      <c r="B11" s="35">
+      <c r="A11" s="22"/>
+      <c r="B11" s="34">
         <f t="shared" ref="B11:B26" si="0">B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="49" t="s">
+      <c r="D11" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="49" t="s">
+      <c r="E11" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="28"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
     </row>
     <row r="12" spans="1:10" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="23"/>
-      <c r="B12" s="35">
+      <c r="A12" s="22"/>
+      <c r="B12" s="34">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="49" t="s">
+      <c r="D12" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="49" t="s">
+      <c r="E12" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="28"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
     </row>
     <row r="13" spans="1:10" ht="35.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="23"/>
-      <c r="B13" s="35">
+      <c r="A13" s="22"/>
+      <c r="B13" s="34">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="48" t="s">
+      <c r="D13" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="49" t="s">
+      <c r="E13" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
     </row>
     <row r="14" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="23"/>
-      <c r="B14" s="35">
+      <c r="A14" s="22"/>
+      <c r="B14" s="34">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
     </row>
     <row r="15" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="23"/>
-      <c r="B15" s="35">
+      <c r="A15" s="22"/>
+      <c r="B15" s="34">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
     </row>
     <row r="16" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="23"/>
-      <c r="B16" s="35">
+      <c r="A16" s="22"/>
+      <c r="B16" s="34">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
     </row>
     <row r="17" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="23"/>
-      <c r="B17" s="35">
+      <c r="A17" s="22"/>
+      <c r="B17" s="34">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
     </row>
     <row r="18" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="23"/>
-      <c r="B18" s="35">
+      <c r="A18" s="22"/>
+      <c r="B18" s="34">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
     </row>
     <row r="19" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="23"/>
-      <c r="B19" s="35">
+      <c r="A19" s="22"/>
+      <c r="B19" s="34">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
     </row>
     <row r="20" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="23"/>
-      <c r="B20" s="35">
+      <c r="A20" s="22"/>
+      <c r="B20" s="34">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
     </row>
     <row r="21" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="23"/>
-      <c r="B21" s="35">
+      <c r="A21" s="22"/>
+      <c r="B21" s="34">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
     </row>
     <row r="22" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="23"/>
-      <c r="B22" s="35">
+      <c r="A22" s="22"/>
+      <c r="B22" s="34">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
     </row>
     <row r="23" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="23"/>
-      <c r="B23" s="35">
+      <c r="A23" s="22"/>
+      <c r="B23" s="34">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
     </row>
     <row r="24" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="23"/>
-      <c r="B24" s="35">
+      <c r="A24" s="22"/>
+      <c r="B24" s="34">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
     </row>
     <row r="25" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="23"/>
-      <c r="B25" s="35">
+      <c r="A25" s="22"/>
+      <c r="B25" s="34">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
     </row>
     <row r="26" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="23"/>
-      <c r="B26" s="35">
+      <c r="A26" s="22"/>
+      <c r="B26" s="34">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
     </row>
     <row r="27" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="22"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
+      <c r="A27" s="21"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
     </row>
     <row r="28" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="22"/>
-      <c r="B28" s="23"/>
-      <c r="C28" s="44" t="s">
+      <c r="A28" s="21"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="45"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -4361,539 +4358,539 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="50" customWidth="1"/>
-    <col min="2" max="2" width="12.36328125" style="50" customWidth="1"/>
-    <col min="3" max="3" width="16.36328125" style="50" customWidth="1"/>
-    <col min="4" max="4" width="18" style="50" customWidth="1"/>
-    <col min="5" max="5" width="41.453125" style="50" customWidth="1"/>
-    <col min="6" max="8" width="8.81640625" style="50" customWidth="1"/>
-    <col min="9" max="9" width="26.6328125" style="50" customWidth="1"/>
-    <col min="10" max="11" width="8.81640625" style="50" customWidth="1"/>
-    <col min="12" max="16384" width="8.81640625" style="50"/>
+    <col min="1" max="1" width="8.81640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="12.36328125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="16.36328125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="18" style="4" customWidth="1"/>
+    <col min="5" max="5" width="41.453125" style="4" customWidth="1"/>
+    <col min="6" max="8" width="8.81640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="26.6328125" style="4" customWidth="1"/>
+    <col min="10" max="11" width="8.81640625" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="8.81640625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20"/>
-      <c r="B1" s="21" t="s">
+      <c r="A1" s="19"/>
+      <c r="B1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="58" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
     </row>
     <row r="2" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="22"/>
-      <c r="B2" s="60" t="s">
+      <c r="A2" s="21"/>
+      <c r="B2" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="25" t="s">
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="J2" s="24" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="25" t="s">
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="25" t="s">
+      <c r="I3" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="25" t="s">
+      <c r="J3" s="24" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="22"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="51" t="s">
+      <c r="A4" s="21"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="72" t="s">
+      <c r="D4" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="73"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="25" t="s">
+      <c r="E4" s="69"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="22"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="51" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="74" t="s">
+      <c r="D5" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="75"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="25" t="s">
+      <c r="E5" s="71"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="25" t="s">
+      <c r="I5" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="25" t="s">
+      <c r="J5" s="24" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="22"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="30" t="s">
+      <c r="A6" s="21"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
     </row>
     <row r="7" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="22"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="30" t="s">
+      <c r="A7" s="21"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
     </row>
     <row r="8" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="22"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
     </row>
     <row r="9" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="23"/>
-      <c r="B9" s="33" t="s">
+      <c r="A9" s="22"/>
+      <c r="B9" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
     </row>
     <row r="10" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="23"/>
-      <c r="B10" s="35">
+      <c r="A10" s="22"/>
+      <c r="B10" s="34">
         <v>1</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="E10" s="42" t="s">
+      <c r="E10" s="41" t="s">
         <v>100</v>
       </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
     </row>
     <row r="11" spans="1:10" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="23"/>
-      <c r="B11" s="35">
+      <c r="A11" s="22"/>
+      <c r="B11" s="34">
         <v>2</v>
       </c>
-      <c r="C11" s="41" t="s">
+      <c r="C11" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="D11" s="41" t="s">
+      <c r="D11" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="E11" s="41" t="s">
         <v>103</v>
       </c>
-      <c r="F11" s="28"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
     </row>
     <row r="12" spans="1:10" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="23"/>
-      <c r="B12" s="35">
+      <c r="A12" s="22"/>
+      <c r="B12" s="34">
         <v>3</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="E12" s="42" t="s">
+      <c r="E12" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="F12" s="28"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
     </row>
     <row r="13" spans="1:10" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="23"/>
-      <c r="B13" s="35">
+      <c r="A13" s="22"/>
+      <c r="B13" s="34">
         <v>4</v>
       </c>
-      <c r="C13" s="41" t="s">
+      <c r="C13" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="D13" s="42" t="s">
+      <c r="D13" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
     </row>
     <row r="14" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="23"/>
-      <c r="B14" s="35">
-        <f t="shared" ref="B11:B30" si="0">B13+1</f>
+      <c r="A14" s="22"/>
+      <c r="B14" s="34">
+        <f t="shared" ref="B14:B30" si="0">B13+1</f>
         <v>5</v>
       </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
     </row>
     <row r="15" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="23"/>
-      <c r="B15" s="35">
+      <c r="A15" s="22"/>
+      <c r="B15" s="34">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
     </row>
     <row r="16" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="23"/>
-      <c r="B16" s="35">
+      <c r="A16" s="22"/>
+      <c r="B16" s="34">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
     </row>
     <row r="17" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="23"/>
-      <c r="B17" s="35">
+      <c r="A17" s="22"/>
+      <c r="B17" s="34">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
     </row>
     <row r="18" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="23"/>
-      <c r="B18" s="35">
+      <c r="A18" s="22"/>
+      <c r="B18" s="34">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
     </row>
     <row r="19" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="23"/>
-      <c r="B19" s="35">
+      <c r="A19" s="22"/>
+      <c r="B19" s="34">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
     </row>
     <row r="20" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="23"/>
-      <c r="B20" s="35">
+      <c r="A20" s="22"/>
+      <c r="B20" s="34">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="41"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
     </row>
     <row r="21" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="23"/>
-      <c r="B21" s="35">
+      <c r="A21" s="22"/>
+      <c r="B21" s="34">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
     </row>
     <row r="22" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="23"/>
-      <c r="B22" s="35">
+      <c r="A22" s="22"/>
+      <c r="B22" s="34">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C22" s="41"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
     </row>
     <row r="23" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="23"/>
-      <c r="B23" s="35">
+      <c r="A23" s="22"/>
+      <c r="B23" s="34">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C23" s="41"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
     </row>
     <row r="24" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="23"/>
-      <c r="B24" s="35">
+      <c r="A24" s="22"/>
+      <c r="B24" s="34">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
     </row>
     <row r="25" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="23"/>
-      <c r="B25" s="35">
+      <c r="A25" s="22"/>
+      <c r="B25" s="34">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C25" s="41"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
     </row>
     <row r="26" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="23"/>
-      <c r="B26" s="35">
+      <c r="A26" s="22"/>
+      <c r="B26" s="34">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
     </row>
     <row r="27" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="23"/>
-      <c r="B27" s="35">
+      <c r="A27" s="22"/>
+      <c r="B27" s="34">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C27" s="41"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
     </row>
     <row r="28" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="23"/>
-      <c r="B28" s="35">
+      <c r="A28" s="22"/>
+      <c r="B28" s="34">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C28" s="41"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
     </row>
     <row r="29" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="23"/>
-      <c r="B29" s="35">
+      <c r="A29" s="22"/>
+      <c r="B29" s="34">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C29" s="41"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="42"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="22"/>
-      <c r="J29" s="22"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
     </row>
     <row r="30" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="23"/>
-      <c r="B30" s="35">
+      <c r="A30" s="22"/>
+      <c r="B30" s="34">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C30" s="41"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="22"/>
-      <c r="J30" s="22"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
     </row>
     <row r="31" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="22"/>
-      <c r="B31" s="31"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="22"/>
-      <c r="J31" s="22"/>
+      <c r="A31" s="21"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
     </row>
     <row r="32" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="22"/>
-      <c r="B32" s="23"/>
-      <c r="C32" s="44" t="s">
+      <c r="A32" s="21"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="45"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="22"/>
-      <c r="J32" s="22"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -4917,575 +4914,575 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A26" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="1.453125" style="52" customWidth="1"/>
-    <col min="2" max="2" width="6.81640625" style="52" customWidth="1"/>
-    <col min="3" max="3" width="21.36328125" style="52" customWidth="1"/>
-    <col min="4" max="4" width="44.1796875" style="52" customWidth="1"/>
-    <col min="5" max="5" width="59.81640625" style="52" customWidth="1"/>
-    <col min="6" max="6" width="59.6328125" style="52" customWidth="1"/>
-    <col min="7" max="8" width="8.81640625" style="52" customWidth="1"/>
-    <col min="9" max="9" width="26.6328125" style="52" customWidth="1"/>
-    <col min="10" max="11" width="8.81640625" style="52" customWidth="1"/>
-    <col min="12" max="16384" width="8.81640625" style="52"/>
+    <col min="1" max="1" width="1.453125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="6.81640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="21.36328125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="44.1796875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="59.81640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="59.6328125" style="4" customWidth="1"/>
+    <col min="7" max="8" width="8.81640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="26.6328125" style="4" customWidth="1"/>
+    <col min="10" max="11" width="8.81640625" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="8.81640625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20"/>
-      <c r="B1" s="21" t="s">
+      <c r="A1" s="19"/>
+      <c r="B1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="58" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
     </row>
     <row r="2" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="22"/>
-      <c r="B2" s="60" t="s">
+      <c r="A2" s="21"/>
+      <c r="B2" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="25" t="s">
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="J2" s="24" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="25" t="s">
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="25" t="s">
+      <c r="I3" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="25" t="s">
+      <c r="J3" s="24" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="22"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="51" t="s">
+      <c r="A4" s="21"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="72" t="s">
+      <c r="D4" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="73"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="25" t="s">
+      <c r="E4" s="69"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="22"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="30" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="68" t="s">
+      <c r="D5" s="64" t="s">
         <v>66</v>
       </c>
-      <c r="E5" s="57"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="25" t="s">
+      <c r="E5" s="53"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="25" t="s">
+      <c r="I5" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="25" t="s">
+      <c r="J5" s="24" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="22"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="30" t="s">
+      <c r="A6" s="21"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="68" t="s">
+      <c r="D6" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="E6" s="57"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
     </row>
     <row r="7" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
     </row>
     <row r="8" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="22"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
     </row>
     <row r="9" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="23"/>
-      <c r="B9" s="33" t="s">
+      <c r="A9" s="22"/>
+      <c r="B9" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="F9" s="33" t="s">
+      <c r="F9" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="G9" s="28"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
     </row>
     <row r="10" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="23"/>
-      <c r="B10" s="35">
+      <c r="A10" s="22"/>
+      <c r="B10" s="34">
         <v>1</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="E10" s="53" t="s">
+      <c r="E10" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="37" t="s">
+      <c r="F10" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="G10" s="28"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
     </row>
     <row r="11" spans="1:10" ht="307" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="23"/>
-      <c r="B11" s="35">
+      <c r="A11" s="22"/>
+      <c r="B11" s="34">
         <f t="shared" ref="B11:B30" si="0">B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="E11" s="37" t="s">
+      <c r="E11" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="F11" s="37" t="s">
+      <c r="F11" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="G11" s="28"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
     </row>
     <row r="12" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="23"/>
-      <c r="B12" s="35">
+      <c r="A12" s="22"/>
+      <c r="B12" s="34">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="36" t="s">
+      <c r="D12" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="E12" s="37" t="s">
+      <c r="E12" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="F12" s="37" t="s">
+      <c r="F12" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="G12" s="28"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
     </row>
     <row r="13" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="23"/>
-      <c r="B13" s="35">
+      <c r="A13" s="22"/>
+      <c r="B13" s="34">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="E13" s="53" t="s">
+      <c r="E13" s="49" t="s">
         <v>86</v>
       </c>
-      <c r="F13" s="37" t="s">
+      <c r="F13" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="G13" s="28"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
     </row>
     <row r="14" spans="1:10" ht="99" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="23"/>
-      <c r="B14" s="35">
+      <c r="A14" s="22"/>
+      <c r="B14" s="34">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="37" t="s">
+      <c r="D14" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="E14" s="37" t="s">
+      <c r="E14" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="F14" s="37" t="s">
+      <c r="F14" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="G14" s="28"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
     </row>
     <row r="15" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="23"/>
-      <c r="B15" s="35">
+      <c r="A15" s="22"/>
+      <c r="B15" s="34">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="37" t="s">
+      <c r="D15" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="E15" s="53" t="s">
+      <c r="E15" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="F15" s="37" t="s">
+      <c r="F15" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="G15" s="28"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
     </row>
     <row r="16" spans="1:10" ht="67" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="23"/>
-      <c r="B16" s="35">
+      <c r="A16" s="22"/>
+      <c r="B16" s="34">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="36" t="s">
+      <c r="C16" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="D16" s="37" t="s">
+      <c r="D16" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="E16" s="37" t="s">
+      <c r="E16" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="F16" s="37" t="s">
+      <c r="F16" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="G16" s="28"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
     </row>
     <row r="17" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="23"/>
-      <c r="B17" s="35">
+      <c r="A17" s="22"/>
+      <c r="B17" s="34">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
     </row>
     <row r="18" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="23"/>
-      <c r="B18" s="35">
+      <c r="A18" s="22"/>
+      <c r="B18" s="34">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
     </row>
     <row r="19" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="23"/>
-      <c r="B19" s="35">
+      <c r="A19" s="22"/>
+      <c r="B19" s="34">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
     </row>
     <row r="20" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="23"/>
-      <c r="B20" s="35">
+      <c r="A20" s="22"/>
+      <c r="B20" s="34">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="41"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
     </row>
     <row r="21" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="23"/>
-      <c r="B21" s="35">
+      <c r="A21" s="22"/>
+      <c r="B21" s="34">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
     </row>
     <row r="22" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="23"/>
-      <c r="B22" s="35">
+      <c r="A22" s="22"/>
+      <c r="B22" s="34">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C22" s="41"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
     </row>
     <row r="23" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="23"/>
-      <c r="B23" s="35">
+      <c r="A23" s="22"/>
+      <c r="B23" s="34">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C23" s="41"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
     </row>
     <row r="24" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="23"/>
-      <c r="B24" s="35">
+      <c r="A24" s="22"/>
+      <c r="B24" s="34">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
     </row>
     <row r="25" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="23"/>
-      <c r="B25" s="35">
+      <c r="A25" s="22"/>
+      <c r="B25" s="34">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C25" s="41"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
     </row>
     <row r="26" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="23"/>
-      <c r="B26" s="35">
+      <c r="A26" s="22"/>
+      <c r="B26" s="34">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
     </row>
     <row r="27" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="23"/>
-      <c r="B27" s="35">
+      <c r="A27" s="22"/>
+      <c r="B27" s="34">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C27" s="41"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
     </row>
     <row r="28" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="23"/>
-      <c r="B28" s="35">
+      <c r="A28" s="22"/>
+      <c r="B28" s="34">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C28" s="41"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
     </row>
     <row r="29" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="23"/>
-      <c r="B29" s="35">
+      <c r="A29" s="22"/>
+      <c r="B29" s="34">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C29" s="41"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="42"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="22"/>
-      <c r="J29" s="22"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
     </row>
     <row r="30" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="23"/>
-      <c r="B30" s="35">
+      <c r="A30" s="22"/>
+      <c r="B30" s="34">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C30" s="41"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="22"/>
-      <c r="J30" s="22"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
     </row>
     <row r="31" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="22"/>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="22"/>
-      <c r="J31" s="22"/>
+      <c r="A31" s="21"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
     </row>
     <row r="32" spans="1:10" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="22"/>
-      <c r="B32" s="23"/>
-      <c r="C32" s="76" t="s">
+      <c r="A32" s="21"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="72" t="s">
         <v>97</v>
       </c>
-      <c r="D32" s="77"/>
-      <c r="E32" s="77"/>
-      <c r="F32" s="54"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="22"/>
-      <c r="J32" s="22"/>
+      <c r="D32" s="73"/>
+      <c r="E32" s="73"/>
+      <c r="F32" s="50"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>